<commit_message>
Adding the new files
</commit_message>
<xml_diff>
--- a/Flags/PolicyGrid/TestDataSheet/Test Data Sheet.xlsx
+++ b/Flags/PolicyGrid/TestDataSheet/Test Data Sheet.xlsx
@@ -1,46 +1,47 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="124226" filterPrivacy="1"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView windowHeight="9825" windowWidth="14025" xWindow="0" yWindow="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14025" windowHeight="9825" activeTab="4"/>
   </bookViews>
   <sheets>
-    <sheet name="241569" r:id="rId1" sheetId="5"/>
-    <sheet name="241570" r:id="rId2" sheetId="14"/>
-    <sheet name="241572" r:id="rId3" sheetId="4"/>
-    <sheet name="241573" r:id="rId4" sheetId="2"/>
-    <sheet name="241575" r:id="rId5" sheetId="6"/>
-    <sheet name="241577" r:id="rId6" sheetId="18"/>
-    <sheet name="245178" r:id="rId7" sheetId="23"/>
-    <sheet name="241579" r:id="rId8" sheetId="3"/>
-    <sheet name="241580" r:id="rId9" sheetId="17"/>
-    <sheet name="241581" r:id="rId10" sheetId="7"/>
-    <sheet name="241582" r:id="rId11" sheetId="8"/>
-    <sheet name="241587" r:id="rId12" sheetId="19"/>
-    <sheet name="255818" r:id="rId13" sheetId="9"/>
-    <sheet name="258900" r:id="rId14" sheetId="15"/>
-    <sheet name="265909" r:id="rId15" sheetId="11"/>
-    <sheet name="258911" r:id="rId16" sheetId="20"/>
-    <sheet name="259848" r:id="rId17" sheetId="24"/>
-    <sheet name="258894" r:id="rId18" sheetId="21"/>
-    <sheet name="265911" r:id="rId19" sheetId="10"/>
-    <sheet name="267971" r:id="rId20" sheetId="16"/>
-    <sheet name="267976" r:id="rId21" sheetId="12"/>
-    <sheet name="267977" r:id="rId22" sheetId="22"/>
-    <sheet name="269079" r:id="rId23" sheetId="13"/>
-    <sheet name="286250" r:id="rId24" sheetId="25"/>
-    <sheet name="295844" r:id="rId25" sheetId="27"/>
-    <sheet name="288245" r:id="rId26" sheetId="28"/>
-    <sheet name="294956" r:id="rId27" sheetId="29"/>
+    <sheet name="241569" sheetId="5" r:id="rId1"/>
+    <sheet name="241570" sheetId="14" r:id="rId2"/>
+    <sheet name="241572" sheetId="4" r:id="rId3"/>
+    <sheet name="241573" sheetId="2" r:id="rId4"/>
+    <sheet name="LinkedIn" sheetId="30" r:id="rId5"/>
+    <sheet name="241575" sheetId="6" r:id="rId6"/>
+    <sheet name="241577" sheetId="18" r:id="rId7"/>
+    <sheet name="245178" sheetId="23" r:id="rId8"/>
+    <sheet name="241579" sheetId="3" r:id="rId9"/>
+    <sheet name="241580" sheetId="17" r:id="rId10"/>
+    <sheet name="241581" sheetId="7" r:id="rId11"/>
+    <sheet name="241582" sheetId="8" r:id="rId12"/>
+    <sheet name="241587" sheetId="19" r:id="rId13"/>
+    <sheet name="255818" sheetId="9" r:id="rId14"/>
+    <sheet name="258900" sheetId="15" r:id="rId15"/>
+    <sheet name="265909" sheetId="11" r:id="rId16"/>
+    <sheet name="258911" sheetId="20" r:id="rId17"/>
+    <sheet name="259848" sheetId="24" r:id="rId18"/>
+    <sheet name="258894" sheetId="21" r:id="rId19"/>
+    <sheet name="265911" sheetId="10" r:id="rId20"/>
+    <sheet name="267971" sheetId="16" r:id="rId21"/>
+    <sheet name="267976" sheetId="12" r:id="rId22"/>
+    <sheet name="267977" sheetId="22" r:id="rId23"/>
+    <sheet name="269079" sheetId="13" r:id="rId24"/>
+    <sheet name="286250" sheetId="25" r:id="rId25"/>
+    <sheet name="295844" sheetId="27" r:id="rId26"/>
+    <sheet name="288245" sheetId="28" r:id="rId27"/>
+    <sheet name="294956" sheetId="29" r:id="rId28"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1615" uniqueCount="369">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1642" uniqueCount="369">
   <si>
     <t>TC_ID</t>
   </si>
@@ -1154,8 +1155,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1268,120 +1268,120 @@
     </border>
   </borders>
   <cellStyleXfs count="4">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="2" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="3" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="39">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="1" fillId="4" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="1" fillId="4" fontId="0" numFmtId="1" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="1" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="1" fillId="4" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" quotePrefix="1" xfId="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="1" fillId="5" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="1" fillId="4" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyBorder="1" borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="3"/>
-    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="6" fontId="4" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="2" fillId="4" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="1" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="1" fillId="4" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="3" fontId="2" numFmtId="0" xfId="2">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" borderId="2" fillId="3" fontId="2" numFmtId="0" xfId="2">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="2" fontId="1" numFmtId="0" quotePrefix="1" xfId="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle builtinId="32" name="60% - Accent1" xfId="2"/>
-    <cellStyle builtinId="26" name="Good" xfId="1"/>
-    <cellStyle builtinId="8" name="Hyperlink" xfId="3"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="60% - Accent1" xfId="2" builtinId="32"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium9" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1398,10 +1398,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -1436,7 +1436,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1471,7 +1471,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1559,7 +1559,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -1568,13 +1568,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1584,7 +1584,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -1593,7 +1593,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1602,7 +1602,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1612,12 +1612,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
+            <a:lightRig rig="threePt" dir="t">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT h="25400" w="63500"/>
+            <a:bevelT w="63500" h="25400"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -1648,7 +1648,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -1667,7 +1667,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -1679,23 +1679,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5:D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" style="20" width="9.140625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="20" width="20.140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="20" width="15.5703125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="20" width="14.85546875" collapsed="true"/>
-    <col min="8" max="16384" style="20" width="9.140625" collapsed="true"/>
+    <col min="1" max="4" width="9.140625" style="20" collapsed="1"/>
+    <col min="5" max="5" width="20.140625" style="20" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.5703125" style="20" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.85546875" style="20" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="16384" width="9.140625" style="20" collapsed="1"/>
   </cols>
   <sheetData>
-    <row ht="30" r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="32" t="s">
         <v>0</v>
       </c>
@@ -1721,7 +1721,7 @@
         <v>355</v>
       </c>
     </row>
-    <row customHeight="1" ht="20.100000000000001" r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>38</v>
       </c>
@@ -1747,7 +1747,7 @@
         <v>364</v>
       </c>
     </row>
-    <row customHeight="1" ht="20.100000000000001" r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
         <v>39</v>
       </c>
@@ -1773,7 +1773,7 @@
         <v>364</v>
       </c>
     </row>
-    <row customHeight="1" ht="20.100000000000001" r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
         <v>40</v>
       </c>
@@ -1797,7 +1797,7 @@
         <v>364</v>
       </c>
     </row>
-    <row customHeight="1" ht="20.100000000000001" r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
         <v>41</v>
       </c>
@@ -1823,7 +1823,7 @@
         <v>364</v>
       </c>
     </row>
-    <row customHeight="1" ht="20.100000000000001" r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
         <v>42</v>
       </c>
@@ -1849,7 +1849,7 @@
         <v>364</v>
       </c>
     </row>
-    <row customHeight="1" ht="20.100000000000001" r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
         <v>43</v>
       </c>
@@ -1875,7 +1875,7 @@
         <v>364</v>
       </c>
     </row>
-    <row customHeight="1" ht="20.100000000000001" r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
         <v>44</v>
       </c>
@@ -1901,7 +1901,7 @@
         <v>364</v>
       </c>
     </row>
-    <row customHeight="1" ht="20.100000000000001" r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
         <v>45</v>
       </c>
@@ -1925,7 +1925,7 @@
         <v>364</v>
       </c>
     </row>
-    <row customHeight="1" ht="20.100000000000001" r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
         <v>46</v>
       </c>
@@ -1951,7 +1951,7 @@
         <v>364</v>
       </c>
     </row>
-    <row customHeight="1" ht="20.100000000000001" r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
         <v>47</v>
       </c>
@@ -1977,7 +1977,7 @@
         <v>364</v>
       </c>
     </row>
-    <row customHeight="1" ht="20.100000000000001" r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="19" t="s">
         <v>48</v>
       </c>
@@ -2001,7 +2001,7 @@
         <v>364</v>
       </c>
     </row>
-    <row customHeight="1" ht="20.100000000000001" r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
         <v>49</v>
       </c>
@@ -2026,13 +2026,201 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H7"/>
+  <sheetViews>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="23.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="28" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="4.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="41.140625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="44.5703125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="92.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="18" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>172</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J1" sqref="J1"/>
@@ -2102,13 +2290,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I5"/>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H1" sqref="H1"/>
@@ -2229,13 +2417,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N24"/>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
@@ -2243,15 +2431,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="35.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="48.42578125" collapsed="true"/>
-    <col min="5" max="6" customWidth="true" width="8.5703125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="6.85546875" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="5.7109375" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="28.0" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="21.85546875" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="19.140625" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="11.42578125" collapsed="true"/>
+    <col min="3" max="3" width="35.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="48.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="6" width="8.5703125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="6.85546875" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="5.7109375" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="28" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="21.85546875" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="19.140625" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="11.42578125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -2295,7 +2483,7 @@
         <v>355</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>38</v>
       </c>
@@ -2326,7 +2514,7 @@
         <v>365</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>39</v>
       </c>
@@ -2357,7 +2545,7 @@
         <v>365</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>40</v>
       </c>
@@ -2388,7 +2576,7 @@
         <v>365</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>41</v>
       </c>
@@ -2419,7 +2607,7 @@
         <v>365</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
         <v>42</v>
       </c>
@@ -2452,7 +2640,7 @@
         <v>365</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
         <v>43</v>
       </c>
@@ -2483,7 +2671,7 @@
         <v>365</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
         <v>44</v>
       </c>
@@ -2514,7 +2702,7 @@
         <v>365</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
         <v>45</v>
       </c>
@@ -2547,7 +2735,7 @@
         <v>365</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
         <v>46</v>
       </c>
@@ -2578,7 +2766,7 @@
         <v>365</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
         <v>47</v>
       </c>
@@ -2611,7 +2799,7 @@
         <v>365</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
         <v>48</v>
       </c>
@@ -2642,7 +2830,7 @@
         <v>365</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
         <v>49</v>
       </c>
@@ -2673,7 +2861,7 @@
         <v>365</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
         <v>56</v>
       </c>
@@ -2704,7 +2892,7 @@
         <v>365</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
         <v>57</v>
       </c>
@@ -2735,7 +2923,7 @@
         <v>365</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
         <v>58</v>
       </c>
@@ -2766,7 +2954,7 @@
         <v>365</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
         <v>59</v>
       </c>
@@ -2797,7 +2985,7 @@
         <v>365</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
         <v>60</v>
       </c>
@@ -2828,7 +3016,7 @@
         <v>365</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
         <v>61</v>
       </c>
@@ -2859,7 +3047,7 @@
         <v>365</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
         <v>62</v>
       </c>
@@ -2894,7 +3082,7 @@
         <v>365</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
         <v>63</v>
       </c>
@@ -2929,7 +3117,7 @@
         <v>365</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="15" t="s">
         <v>64</v>
       </c>
@@ -2960,7 +3148,7 @@
         <v>365</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="15" t="s">
         <v>65</v>
       </c>
@@ -2991,7 +3179,7 @@
         <v>365</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="15" t="s">
         <v>66</v>
       </c>
@@ -3024,16 +3212,16 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="G24"/>
+    <hyperlink ref="G24" r:id="rId1"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H80"/>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G80"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G1" sqref="G1"/>
@@ -3041,8 +3229,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="35.5703125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="28.0" collapsed="true"/>
+    <col min="2" max="2" width="35.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="28" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -4649,13 +4837,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H3"/>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G1" sqref="G1"/>
@@ -4686,7 +4874,7 @@
         <v>355</v>
       </c>
     </row>
-    <row customHeight="1" ht="20.100000000000001" r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>38</v>
       </c>
@@ -4709,7 +4897,7 @@
         <v>366</v>
       </c>
     </row>
-    <row customHeight="1" ht="20.100000000000001" r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>39</v>
       </c>
@@ -4733,13 +4921,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M2"/>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="L1" sqref="L1"/>
@@ -4747,8 +4935,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="35.5703125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="19.42578125" collapsed="true"/>
+    <col min="2" max="2" width="35.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -4819,13 +5007,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H5"/>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="G1" sqref="G1"/>
@@ -4833,10 +5021,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="6.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="4.42578125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="92.5703125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="83.5703125" collapsed="true"/>
+    <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="4.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="92.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="83.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -4862,7 +5050,7 @@
         <v>355</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>38</v>
       </c>
@@ -4882,7 +5070,7 @@
         <v>263</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>39</v>
       </c>
@@ -4902,7 +5090,7 @@
         <v>266</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>40</v>
       </c>
@@ -4922,7 +5110,7 @@
         <v>268</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>41</v>
       </c>
@@ -4943,13 +5131,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I4"/>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H1" sqref="H1"/>
@@ -4957,7 +5145,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="58.42578125" collapsed="true"/>
+    <col min="6" max="6" width="58.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -5044,13 +5232,13 @@
       <c r="G4" s="15"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J3"/>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView topLeftCell="G1" workbookViewId="0">
       <selection activeCell="I1" sqref="I1"/>
@@ -5058,13 +5246,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="6.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="45.28515625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="23.7109375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="4.42578125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="85.7109375" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="62.140625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="65.7109375" collapsed="true"/>
+    <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="45.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="23.7109375" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="4.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="85.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="62.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="65.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -5096,7 +5284,7 @@
         <v>355</v>
       </c>
     </row>
-    <row customHeight="1" ht="20.100000000000001" r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>282</v>
       </c>
@@ -5122,7 +5310,7 @@
         <v>280</v>
       </c>
     </row>
-    <row customHeight="1" ht="20.100000000000001" r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>283</v>
       </c>
@@ -5149,96 +5337,23 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" customWidth="true" width="8.85546875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="20.140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="15.5703125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>336</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="F1" s="25" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row customFormat="1" ht="135" r="2" s="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="29" t="s">
-        <v>38</v>
-      </c>
-      <c r="B2" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="30" t="s">
-        <v>123</v>
-      </c>
-      <c r="D2" s="29" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="29" t="s">
-        <v>319</v>
-      </c>
-      <c r="F2" s="29" t="s">
-        <v>320</v>
-      </c>
-      <c r="G2" s="29" t="s">
-        <v>321</v>
-      </c>
-      <c r="H2" t="s">
-        <v>364</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M92"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L92"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="64" zoomScaleNormal="64">
+    <sheetView zoomScale="64" zoomScaleNormal="64" workbookViewId="0">
       <selection activeCell="J2" sqref="J2:J92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="35.5703125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="56.140625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="28.0" collapsed="true"/>
+    <col min="2" max="2" width="35.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="56.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="28" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -7358,13 +7473,86 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="8.85546875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="31" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+      <c r="A2" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="30" t="s">
+        <v>123</v>
+      </c>
+      <c r="D2" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="29" t="s">
+        <v>319</v>
+      </c>
+      <c r="F2" s="29" t="s">
+        <v>320</v>
+      </c>
+      <c r="G2" s="29" t="s">
+        <v>321</v>
+      </c>
+      <c r="H2" t="s">
+        <v>364</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
@@ -7372,10 +7560,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="35.5703125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="28.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="20.140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="113.85546875" collapsed="true"/>
+    <col min="2" max="2" width="35.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="28" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="113.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -7404,7 +7592,7 @@
         <v>355</v>
       </c>
     </row>
-    <row customHeight="1" ht="18" r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>38</v>
       </c>
@@ -7430,7 +7618,7 @@
         <v>364</v>
       </c>
     </row>
-    <row customHeight="1" ht="18" r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>39</v>
       </c>
@@ -7457,13 +7645,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J2"/>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I1" sqref="I1"/>
@@ -7527,13 +7715,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
@@ -7541,10 +7729,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="6.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="4.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="23.7109375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="4.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="23.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -7593,14 +7781,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J2"/>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I1" sqref="I1"/>
@@ -7664,13 +7852,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H1" sqref="H1"/>
@@ -7678,7 +7866,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="101.42578125" collapsed="true"/>
+    <col min="7" max="7" width="101.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -7754,13 +7942,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L5"/>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K1" sqref="K1"/>
@@ -7768,7 +7956,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="23.7109375" collapsed="true"/>
+    <col min="2" max="2" width="23.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -7915,13 +8103,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I2"/>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H1" sqref="H1"/>
@@ -7979,13 +8167,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I2"/>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="L12" sqref="L12"/>
@@ -8043,13 +8231,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2:D4"/>
@@ -8057,11 +8245,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="20" width="15.5703125" collapsed="true"/>
-    <col min="2" max="16384" style="20" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="15.5703125" style="20" customWidth="1" collapsed="1"/>
+    <col min="2" max="16384" width="9.140625" style="20" collapsed="1"/>
   </cols>
   <sheetData>
-    <row ht="60" r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
@@ -8090,7 +8278,7 @@
         <v>355</v>
       </c>
     </row>
-    <row customHeight="1" ht="20.100000000000001" r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="36" t="s">
         <v>38</v>
       </c>
@@ -8117,7 +8305,7 @@
         <v>364</v>
       </c>
     </row>
-    <row customHeight="1" ht="20.100000000000001" r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="36" t="s">
         <v>39</v>
       </c>
@@ -8144,7 +8332,7 @@
         <v>364</v>
       </c>
     </row>
-    <row customHeight="1" ht="20.100000000000001" r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="36" t="s">
         <v>40</v>
       </c>
@@ -8174,28 +8362,28 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0" zoomScale="69" zoomScaleNormal="69">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView topLeftCell="A3" zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
+      <selection activeCell="C3" sqref="A1:I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="20" width="16.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="20" width="35.5703125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="20" width="60.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="20" width="28.0" collapsed="true"/>
-    <col min="5" max="16384" style="20" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="16.5703125" style="20" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="35.5703125" style="20" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="60.28515625" style="20" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="28" style="20" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="16384" width="9.140625" style="20" collapsed="1"/>
   </cols>
   <sheetData>
-    <row ht="60" r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
@@ -8224,7 +8412,7 @@
         <v>355</v>
       </c>
     </row>
-    <row ht="210" r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="210" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
         <v>38</v>
       </c>
@@ -8251,7 +8439,7 @@
         <v>364</v>
       </c>
     </row>
-    <row ht="315" r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="315" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
         <v>39</v>
       </c>
@@ -8280,7 +8468,7 @@
         <v>365</v>
       </c>
     </row>
-    <row ht="285" r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="285" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
         <v>40</v>
       </c>
@@ -8310,13 +8498,142 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="18" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="210" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="38" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="315" x14ac:dyDescent="0.25">
+      <c r="A3" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>367</v>
+      </c>
+      <c r="F3" s="38" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="38" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="285" x14ac:dyDescent="0.25">
+      <c r="A4" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="38" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="38" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" s="38" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" t="s">
+        <v>365</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
@@ -8324,12 +8641,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="87.7109375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="123.5703125" collapsed="true"/>
+    <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="87.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="123.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row ht="60" r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -8422,13 +8739,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N4"/>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="M4" sqref="M4"/>
@@ -8436,8 +8753,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="35.5703125" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="20" width="44.85546875" collapsed="true"/>
+    <col min="2" max="2" width="35.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="44.85546875" style="20" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -8481,7 +8798,7 @@
         <v>355</v>
       </c>
     </row>
-    <row customHeight="1" ht="20.100000000000001" r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>38</v>
       </c>
@@ -8519,7 +8836,7 @@
         <v>181</v>
       </c>
     </row>
-    <row customHeight="1" ht="20.100000000000001" r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>39</v>
       </c>
@@ -8551,7 +8868,7 @@
         <v>182</v>
       </c>
     </row>
-    <row customHeight="1" ht="20.100000000000001" r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>40</v>
       </c>
@@ -8584,13 +8901,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K3"/>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J1" sqref="J1"/>
@@ -8685,13 +9002,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K2"/>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView topLeftCell="I1" workbookViewId="0">
       <selection activeCell="J1" sqref="J1"/>
@@ -8699,14 +9016,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="16.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="35.5703125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="28.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="28.0" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="4.42578125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="95.42578125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="99.0" collapsed="true"/>
+    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="35.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="28" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="28" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="4.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="95.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="99" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -8774,194 +9091,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I7"/>
-  <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="16.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="23.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="28.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="4.42578125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="41.140625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="44.5703125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="92.42578125" collapsed="true"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H1" s="18" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>167</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>167</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>168</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>168</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>170</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>170</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>171</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>171</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>172</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>172</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>172</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>